<commit_message>
Más comentarios para el ejercicio 1 y el ejercicio 2 del taller final.
</commit_message>
<xml_diff>
--- a/practicaPOO/tallerFinal/Ejercicio1/estudiantes.xlsx
+++ b/practicaPOO/tallerFinal/Ejercicio1/estudiantes.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -441,7 +441,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>David Darquea</t>
+          <t>David</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -450,22 +450,7 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>Marcos Rodriguez</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>Ingeniería Industrial</t>
-        </is>
-      </c>
-      <c r="C3" t="n">
-        <v>15</v>
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>